<commit_message>
ran update - now even with "Last updated 10:00 am, 25 March 2020"
</commit_message>
<xml_diff>
--- a/data/cases-regions.xlsx
+++ b/data/cases-regions.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -418,10 +418,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -574,7 +574,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Southland</t>
+          <t>South Canterbury</t>
         </is>
       </c>
       <c r="B14">
@@ -590,16 +590,32 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>Southland</t>
+        </is>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>Tasman</t>
         </is>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update "Last updated 2:00 pm, 25 March 2020"
</commit_message>
<xml_diff>
--- a/data/cases-regions.xlsx
+++ b/data/cases-regions.xlsx
@@ -386,10 +386,10 @@
         </is>
       </c>
       <c r="B2">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="C2">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -402,10 +402,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C3">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D3">
         <v>4</v>
@@ -418,10 +418,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C4">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -434,10 +434,10 @@
         </is>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -450,10 +450,10 @@
         </is>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -462,23 +462,23 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Nelson</t>
+          <t>Marlborough</t>
         </is>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Taranaki</t>
+          <t>Nelson</t>
         </is>
       </c>
       <c r="B8">
@@ -494,14 +494,14 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Marlborough</t>
+          <t>Taranaki</t>
         </is>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -510,7 +510,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Hawke’s Bay</t>
+          <t>Bay of Plenty</t>
         </is>
       </c>
       <c r="B10">
@@ -526,7 +526,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Manawatu-Whanganui</t>
+          <t>Hawke’s Bay</t>
         </is>
       </c>
       <c r="B11">
@@ -542,14 +542,14 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Bay of Plenty</t>
+          <t>Manawatu-Whanganui</t>
         </is>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -574,17 +574,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>South Canterbury</t>
+          <t>TBC</t>
         </is>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">

</xml_diff>